<commit_message>
Atualização da lista com o requisito Banana
</commit_message>
<xml_diff>
--- a/PastaDocumentosRequisitos/ListaRequisitos-CASE.xlsx
+++ b/PastaDocumentosRequisitos/ListaRequisitos-CASE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DataGov\FIAP-DataGovernance-Aula-4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonpflocal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D6D6209-2EF7-4501-B984-6BD977AAC50A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEF5A19-50A6-4FD5-90FF-FEDD2E3468EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7545" xr2:uid="{9644AAFF-B33B-4270-B576-8A6919809027}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>REQUISITO</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Cada cliente só visualiza os seus pontos</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -480,7 +486,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,11 +609,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>

</xml_diff>